<commit_message>
Updated integration test results
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/ms6/Test Report MS6.xlsx
+++ b/Documents/Testing/TestsDocuments/ms6/Test Report MS6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicole Chan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zohrab Zeynalli\OneDrive\Documents\SENECA\2semester\SFT221\SFT221_GROUP_PROJECT\Documents\Testing\TestsDocuments\ms6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A244B71-2A16-49EE-8489-360C74E74CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B06BA3-6A68-4CB8-A355-F36A380C78A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{14A4F91B-D742-415A-99CE-6B406179EB69}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{14A4F91B-D742-415A-99CE-6B406179EB69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -420,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -434,10 +434,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -447,23 +444,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -781,14 +775,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD8AF7A-AFF9-47BB-B802-9533E9C75ED8}">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="58.77734375" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" style="1" customWidth="1"/>
     <col min="5" max="5" width="48.77734375" style="1" customWidth="1"/>
@@ -813,7 +807,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="13" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -822,109 +816,109 @@
       <c r="C2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="5" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
-      <c r="B11" s="11"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -932,7 +926,7 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -941,133 +935,133 @@
       <c r="C12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="9"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
-      <c r="B23" s="11"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1075,7 +1069,7 @@
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -1084,205 +1078,205 @@
       <c r="C24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="8" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="8" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="8" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="9"/>
+      <c r="A32" s="13"/>
       <c r="B32" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="8" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
+      <c r="A33" s="13"/>
       <c r="B33" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="9"/>
+      <c r="A35" s="13"/>
       <c r="B35" s="5" t="s">
         <v>54</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="9"/>
+      <c r="A36" s="13"/>
       <c r="B36" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="9"/>
+      <c r="A37" s="13"/>
       <c r="B37" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="9"/>
+      <c r="A38" s="13"/>
       <c r="B38" s="5" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="9"/>
+      <c r="A39" s="13"/>
       <c r="B39" s="5" t="s">
         <v>58</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D39" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D39" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
-      <c r="B40" s="11"/>
+      <c r="B40" s="9"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -1290,7 +1284,7 @@
       <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="12" t="s">
         <v>49</v>
       </c>
       <c r="B41" s="5" t="s">
@@ -1299,121 +1293,121 @@
       <c r="C41" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="6"/>
+      <c r="A42" s="12"/>
       <c r="B42" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="6"/>
+      <c r="A43" s="12"/>
       <c r="B43" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="6"/>
+      <c r="A44" s="12"/>
       <c r="B44" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="6"/>
+      <c r="A45" s="12"/>
       <c r="B45" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="6"/>
+      <c r="A46" s="12"/>
       <c r="B46" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="6"/>
+      <c r="A47" s="12"/>
       <c r="B47" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="6"/>
+      <c r="A48" s="12"/>
       <c r="B48" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="6"/>
+      <c r="A49" s="12"/>
       <c r="B49" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="6"/>
+      <c r="A50" s="12"/>
       <c r="B50" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D50" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D50" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
-      <c r="B51" s="11"/>
+      <c r="B51" s="9"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -1421,7 +1415,7 @@
       <c r="G51" s="2"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="10" t="s">
+      <c r="A52" s="8" t="s">
         <v>50</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -1430,13 +1424,13 @@
       <c r="C52" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D52" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D52" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
-      <c r="B53" s="11"/>
+      <c r="B53" s="9"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -1444,7 +1438,7 @@
       <c r="G53" s="2"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="10" t="s">
+      <c r="A54" s="8" t="s">
         <v>51</v>
       </c>
       <c r="B54" s="5" t="s">
@@ -1453,13 +1447,13 @@
       <c r="C54" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D54" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D54" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
-      <c r="B55" s="13"/>
+      <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -1467,166 +1461,166 @@
       <c r="G55" s="2"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="11" t="s">
         <v>67</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="D56" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="6"/>
-      <c r="B57" s="15" t="s">
+      <c r="A57" s="12"/>
+      <c r="B57" s="11" t="s">
         <v>68</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D57" s="8" t="s">
+      <c r="D57" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="6"/>
-      <c r="B58" s="15" t="s">
+      <c r="A58" s="12"/>
+      <c r="B58" s="11" t="s">
         <v>69</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D58" s="8" t="s">
+      <c r="D58" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="6"/>
-      <c r="B59" s="15" t="s">
+      <c r="A59" s="12"/>
+      <c r="B59" s="11" t="s">
         <v>70</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D59" s="8" t="s">
+      <c r="D59" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="6"/>
-      <c r="B60" s="15" t="s">
+      <c r="A60" s="12"/>
+      <c r="B60" s="11" t="s">
         <v>71</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D60" s="8" t="s">
+      <c r="D60" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="6"/>
-      <c r="B61" s="15" t="s">
+      <c r="A61" s="12"/>
+      <c r="B61" s="11" t="s">
         <v>72</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="D61" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="6"/>
-      <c r="B62" s="15" t="s">
+      <c r="A62" s="12"/>
+      <c r="B62" s="11" t="s">
         <v>73</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="D62" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="6"/>
-      <c r="B63" s="15" t="s">
+      <c r="A63" s="12"/>
+      <c r="B63" s="11" t="s">
         <v>74</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D63" s="8" t="s">
+      <c r="D63" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="6"/>
-      <c r="B64" s="15" t="s">
+      <c r="A64" s="12"/>
+      <c r="B64" s="11" t="s">
         <v>75</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="D64" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="6"/>
-      <c r="B65" s="15" t="s">
+      <c r="A65" s="12"/>
+      <c r="B65" s="11" t="s">
         <v>77</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D65" s="8" t="s">
+      <c r="D65" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="6"/>
-      <c r="B66" s="15" t="s">
+      <c r="A66" s="12"/>
+      <c r="B66" s="11" t="s">
         <v>78</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D66" s="8" t="s">
+      <c r="D66" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="6"/>
-      <c r="B67" s="15" t="s">
+      <c r="A67" s="12"/>
+      <c r="B67" s="11" t="s">
         <v>79</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D67" s="8" t="s">
+      <c r="D67" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="6"/>
-      <c r="B68" s="15" t="s">
+      <c r="A68" s="12"/>
+      <c r="B68" s="11" t="s">
         <v>80</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D68" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D68" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
-      <c r="B69" s="13"/>
+      <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -1634,160 +1628,160 @@
       <c r="G69" s="2"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="6" t="s">
+      <c r="A70" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B70" s="15" t="s">
+      <c r="B70" s="11" t="s">
         <v>81</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="D70" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="6"/>
-      <c r="B71" s="15" t="s">
+      <c r="A71" s="12"/>
+      <c r="B71" s="11" t="s">
         <v>82</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D71" s="8" t="s">
+      <c r="D71" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="6"/>
-      <c r="B72" s="15" t="s">
+      <c r="A72" s="12"/>
+      <c r="B72" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D72" s="8" t="s">
+      <c r="D72" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="6"/>
-      <c r="B73" s="15" t="s">
+      <c r="A73" s="12"/>
+      <c r="B73" s="11" t="s">
         <v>84</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D73" s="8" t="s">
+      <c r="D73" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="6"/>
-      <c r="B74" s="15" t="s">
+      <c r="A74" s="12"/>
+      <c r="B74" s="11" t="s">
         <v>85</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D74" s="8" t="s">
+      <c r="D74" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="6"/>
-      <c r="B75" s="15" t="s">
+      <c r="A75" s="12"/>
+      <c r="B75" s="11" t="s">
         <v>86</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D75" s="8" t="s">
+      <c r="D75" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="6"/>
-      <c r="B76" s="15" t="s">
+      <c r="A76" s="12"/>
+      <c r="B76" s="11" t="s">
         <v>87</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D76" s="8" t="s">
+      <c r="D76" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" s="6"/>
-      <c r="B77" s="15" t="s">
+      <c r="A77" s="12"/>
+      <c r="B77" s="11" t="s">
         <v>88</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D77" s="8" t="s">
+      <c r="D77" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A78" s="6"/>
-      <c r="B78" s="15" t="s">
+      <c r="A78" s="12"/>
+      <c r="B78" s="11" t="s">
         <v>89</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D78" s="8" t="s">
+      <c r="D78" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A79" s="6"/>
-      <c r="B79" s="15" t="s">
+      <c r="A79" s="12"/>
+      <c r="B79" s="11" t="s">
         <v>92</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D79" s="8" t="s">
+      <c r="D79" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" s="6"/>
-      <c r="B80" s="15" t="s">
+      <c r="A80" s="12"/>
+      <c r="B80" s="11" t="s">
         <v>93</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D80" s="8" t="s">
+      <c r="D80" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="6"/>
-      <c r="B81" s="15" t="s">
+      <c r="A81" s="12"/>
+      <c r="B81" s="11" t="s">
         <v>94</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D81" s="8" t="s">
+      <c r="D81" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="6"/>
-      <c r="B82" s="15" t="s">
+      <c r="A82" s="12"/>
+      <c r="B82" s="11" t="s">
         <v>95</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D82" s="8" t="s">
+      <c r="D82" s="7" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>